<commit_message>
Set cwl parameters to be read from parameters file
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="hydro" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="channel" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">NDAYS</t>
   </si>
@@ -51,6 +52,45 @@
   </si>
   <si>
     <t xml:space="preserve">n_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">block_height_from_surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">block_coeff_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_ini_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_ini_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel_bottom_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_BC_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5</t>
   </si>
 </sst>
 </file>
@@ -150,8 +190,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,19 +294,19 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>364</v>
       </c>
     </row>
@@ -285,272 +329,272 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="F2" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="C3" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>7.5</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="F3" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="2" t="n">
+      <c r="C4" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>500</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="F4" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="C5" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>500</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>7.5</v>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="F5" s="3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C6" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>2.5</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="F6" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="3" t="n">
+      <c r="C7" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>7.5</v>
       </c>
-      <c r="F7" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="F7" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="C8" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="4" t="n">
+      <c r="C8" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="5" t="n">
         <v>500</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>2.5</v>
       </c>
-      <c r="F8" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G8" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="F8" s="5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="5" t="n">
         <v>500</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="5" t="n">
         <v>7.5</v>
       </c>
-      <c r="F9" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="n">
+      <c r="F9" s="5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -563,4 +607,80 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
saving in case battery goes off
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -298,7 +298,7 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -332,9 +332,9 @@
       <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,10 +617,10 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
   </cols>

</xml_diff>

<commit_message>
added cwl hydro params to be read from file
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">NDAYS</t>
   </si>
@@ -42,6 +42,30 @@
     <t xml:space="preserve">t2</t>
   </si>
   <si>
+    <t xml:space="preserve">block_height_from_surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">block_coeff_k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_ini_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_ini_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel_bottom_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y_BC_below_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel_width</t>
+  </si>
+  <si>
     <t xml:space="preserve">porous_threshold</t>
   </si>
   <si>
@@ -54,28 +78,10 @@
     <t xml:space="preserve">n_threshold</t>
   </si>
   <si>
-    <t xml:space="preserve">block_height_from_surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">block_coeff_k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y_ini_below_DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q_ini_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">channel_bottom_below_DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y_BC_below_DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">channel_width</t>
+    <t xml:space="preserve">max_niter_newton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_niter_newton_inexact</t>
   </si>
   <si>
     <t xml:space="preserve">0.0</t>
@@ -124,7 +130,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +159,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F0D9"/>
         <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCC9C8"/>
+        <bgColor rgb="FFFBE5D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999966"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -190,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +230,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,7 +299,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFCC9C8"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -273,7 +307,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999966"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -298,7 +332,7 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -326,13 +360,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
   </cols>
@@ -353,18 +387,6 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -382,18 +404,6 @@
       <c r="E2" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -411,18 +421,6 @@
       <c r="E3" s="2" t="n">
         <v>7.5</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -440,18 +438,6 @@
       <c r="E4" s="3" t="n">
         <v>2.5</v>
       </c>
-      <c r="F4" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -469,18 +455,6 @@
       <c r="E5" s="3" t="n">
         <v>7.5</v>
       </c>
-      <c r="F5" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -498,18 +472,6 @@
       <c r="E6" s="4" t="n">
         <v>2.5</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -527,18 +489,6 @@
       <c r="E7" s="4" t="n">
         <v>7.5</v>
       </c>
-      <c r="F7" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -556,18 +506,6 @@
       <c r="E8" s="5" t="n">
         <v>2.5</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -584,18 +522,6 @@
       </c>
       <c r="E9" s="5" t="n">
         <v>7.5</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -614,64 +540,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="H1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="L1" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>22</v>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J2" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added peat hydro params to external file
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="hydro" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="peat_hydro_prop" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="channel" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="peat" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t xml:space="preserve">NDAYS</t>
   </si>
@@ -97,6 +98,15 @@
   </si>
   <si>
     <t xml:space="preserve">3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_sweeps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fipy_desired_residual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00001</t>
   </si>
 </sst>
 </file>
@@ -332,7 +342,7 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -366,7 +376,7 @@
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
   </cols>
@@ -542,13 +552,15 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,6 +647,50 @@
       </c>
       <c r="N2" s="0" t="n">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.35"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added zeta diri BC to external parameter
</commit_message>
<xml_diff>
--- a/2d_calibration_parameters.xlsx
+++ b/2d_calibration_parameters.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">NDAYS</t>
   </si>
@@ -106,7 +106,13 @@
     <t xml:space="preserve">fipy_desired_residual</t>
   </si>
   <si>
+    <t xml:space="preserve">zeta_diri_BC</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.2</t>
   </si>
 </sst>
 </file>
@@ -665,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,13 +690,19 @@
       <c r="B1" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>